<commit_message>
Adding the workshop results
</commit_message>
<xml_diff>
--- a/org.panorama-research.waters-2019.hazards/waters-challenge-hazards.xlsx
+++ b/org.panorama-research.waters-2019.hazards/waters-challenge-hazards.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,64 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="465" windowWidth="23265" windowHeight="12585"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hazards" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Bjoern Koopmann</author>
-  </authors>
-  <commentList>
-    <comment ref="E2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Bjoern Koopmann:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Move column in other file (not part of hazard analysis)?</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Hazard</t>
   </si>
@@ -74,9 +32,6 @@
     <t>Accidental event (what, where, when)</t>
   </si>
   <si>
-    <t>Preventive actions</t>
-  </si>
-  <si>
     <t>Severity</t>
   </si>
   <si>
@@ -86,9 +41,6 @@
     <t>Probable causes</t>
   </si>
   <si>
-    <t>Redundant sensors and actuators; high integrity ECU operation</t>
-  </si>
-  <si>
     <t>S3</t>
   </si>
   <si>
@@ -119,29 +71,53 @@
     <t>C</t>
   </si>
   <si>
-    <t>While driving, the vehicle is not able to stop in time to avoid a collision with a vulnerable road user and hits the vulnerable road user</t>
-  </si>
-  <si>
     <t>Sensor failure in the detection of obstacles; ECU failure; failure of the break actuator</t>
   </si>
   <si>
-    <t>Collision with vulnerable road user</t>
-  </si>
-  <si>
-    <t>While driving, the vehicle suddenly stops although no obstacle is in front of the vehicle; vehicles following directly behing might crash into the vehicle</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
     <t>Exposure</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Sensor failure; erroneous calculation of speed profile; erroneous identification of the driving situation; wrong detection of traffic signs; failure of the motor control</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Collision with an obstacle (static obstacle or road user)</t>
+  </si>
+  <si>
+    <t>Unintended acceleration</t>
+  </si>
+  <si>
+    <t>Unintended leaving of the road</t>
+  </si>
+  <si>
+    <t>While driving, the vehicle is not able to stop in time to avoid a collision with a road user or a static obstacle and hits the road user or static obstacle.</t>
+  </si>
+  <si>
+    <t>While driving, the vehicle suddenly stops although no obstacle is in front of the vehicle; vehicles following directly behing might crash into the vehicle.</t>
+  </si>
+  <si>
+    <t>While driving, the vehicle suddenly accerates without any reason and can collide with an obstacle on or offside the road.</t>
+  </si>
+  <si>
+    <t>While driving, the vehicle is  following a wrong trajectory and leaves the road and may hit an obstacle.</t>
+  </si>
+  <si>
+    <t>Sensor or actuator failures; misinterpretation of sensor signals; wrong localization; wrong classification of the road; erroneous trajactory planning; ECU failure; wrong timing of steering command</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,19 +132,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -212,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -235,6 +198,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,11 +515,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,14 +527,13 @@
     <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -577,117 +542,137 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>19</v>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="H3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>9</v>
-      </c>
       <c r="G4" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -695,9 +680,8 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -706,9 +690,8 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -717,9 +700,8 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -728,9 +710,8 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -739,9 +720,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -750,9 +730,8 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -761,11 +740,9 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating the hazard IDs
</commit_message>
<xml_diff>
--- a/org.panorama-research.waters-2019.hazards/waters-challenge-hazards.xlsx
+++ b/org.panorama-research.waters-2019.hazards/waters-challenge-hazards.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Hazard</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>Sensor or actuator failures; misinterpretation of sensor signals; wrong localization; wrong classification of the road; erroneous trajactory planning; controller failure; wrong timing of steering command</t>
+  </si>
+  <si>
+    <t>H-1</t>
+  </si>
+  <si>
+    <t>H-2</t>
+  </si>
+  <si>
+    <t>H-3</t>
+  </si>
+  <si>
+    <t>H-4</t>
   </si>
 </sst>
 </file>
@@ -175,17 +187,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -198,9 +206,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,230 +521,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H14"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="3" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor corrections and updates
</commit_message>
<xml_diff>
--- a/org.panorama-research.waters-2019.hazards/waters-challenge-hazards.xlsx
+++ b/org.panorama-research.waters-2019.hazards/waters-challenge-hazards.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hazards" sheetId="1" r:id="rId1"/>
+    <sheet name="Assumptions" sheetId="2" r:id="rId1"/>
+    <sheet name="Hazards" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Hazard</t>
   </si>
@@ -101,9 +102,6 @@
     <t>While driving, the vehicle suddenly stops although no obstacle is in front of the vehicle; vehicles following directly behing might crash into the vehicle.</t>
   </si>
   <si>
-    <t>While driving, the vehicle suddenly accerates without any reason and can collide with an obstacle on or offside the road.</t>
-  </si>
-  <si>
     <t>While driving, the vehicle is  following a wrong trajectory and leaves the road and may hit an obstacle.</t>
   </si>
   <si>
@@ -123,6 +121,45 @@
   </si>
   <si>
     <t>H-4</t>
+  </si>
+  <si>
+    <t>A-1</t>
+  </si>
+  <si>
+    <t>A-2</t>
+  </si>
+  <si>
+    <t>A-1.1</t>
+  </si>
+  <si>
+    <t>A-3</t>
+  </si>
+  <si>
+    <t>The vehicle has an SAE automation level of 3.</t>
+  </si>
+  <si>
+    <t>The vehicle is used exclusively in urban areas.</t>
+  </si>
+  <si>
+    <t>The vehicle has a normal braking distance of (speed [km/h] / 10)^2.</t>
+  </si>
+  <si>
+    <t>The vehicle has an emergency braking distance of (speed [km/h] / 10)^2 / 2.</t>
+  </si>
+  <si>
+    <t>A-4</t>
+  </si>
+  <si>
+    <t>A-5</t>
+  </si>
+  <si>
+    <t>The vehicle has a minimum (front) sensing range of 100 m.</t>
+  </si>
+  <si>
+    <t>The vehicle drives at a maximum speed of 50 km/h (~ 13.89 m/s).</t>
+  </si>
+  <si>
+    <t>While driving, the vehicle suddenly accelerates without any reason and can collide with an obstacle on or offside the road.</t>
   </si>
 </sst>
 </file>
@@ -187,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -207,6 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -521,11 +559,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="69" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -564,7 +667,7 @@
     </row>
     <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>20</v>
@@ -573,7 +676,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>8</v>
@@ -590,7 +693,7 @@
     </row>
     <row r="3" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -599,7 +702,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>7</v>
@@ -616,13 +719,13 @@
     </row>
     <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>18</v>
@@ -642,16 +745,16 @@
     </row>
     <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>7</v>

</xml_diff>